<commit_message>
Actualizacion de los diagramas de gantt para que el tamaño de las etiquetas sea mas grande
</commit_message>
<xml_diff>
--- a/Informe/Diagrama de Gantt/Diagrama de Gantt.xlsx
+++ b/Informe/Diagrama de Gantt/Diagrama de Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico Albertengo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001306F0-493E-40FB-AD91-F0027485AC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9E3B8E-7DD6-4CDF-9DDD-94C18D732286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{5FAFB7AC-6A9B-44A5-84CE-094E9B5C40EE}"/>
   </bookViews>
@@ -1641,7 +1641,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1713,7 +1713,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2110,6 +2110,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2132,7 +2146,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2204,7 +2218,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2220,7 +2234,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="186351327"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -2666,7 +2680,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2738,7 +2752,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3133,7 +3147,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3205,7 +3219,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3636,7 +3650,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3708,7 +3722,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -7143,8 +7157,8 @@
       <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>5332</xdr:rowOff>
     </xdr:to>
@@ -7181,13 +7195,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>219074</xdr:colOff>
+      <xdr:colOff>219073</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>5332</xdr:rowOff>
     </xdr:to>
@@ -7229,8 +7243,8 @@
       <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>5332</xdr:rowOff>
     </xdr:to>
@@ -8392,7 +8406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F541D4-632E-4CF3-82CA-982F795E8F2A}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" workbookViewId="0">
+    <sheetView topLeftCell="C4" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -8727,7 +8741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B17453-26BC-47A2-BB64-4A12FA0B0C8A}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="I4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -9134,8 +9148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AB6520-4DE5-4B14-9F96-39D8B449A877}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD23" sqref="AD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9570,7 +9584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5DAE94-0AAC-4B00-83DE-A038FBD6DF23}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -9964,7 +9978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C040AA46-4824-499A-AC6B-49AC956C6EE1}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corregidos diagramas de gantt de la iteración 1 y 2
</commit_message>
<xml_diff>
--- a/Informe/Diagrama de Gantt/Diagrama de Gantt.xlsx
+++ b/Informe/Diagrama de Gantt/Diagrama de Gantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico Albertengo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Conferentia\Informe\Diagrama de Gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9E3B8E-7DD6-4CDF-9DDD-94C18D732286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A2898A-8E9A-4C44-914D-320710E08A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{5FAFB7AC-6A9B-44A5-84CE-094E9B5C40EE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{5FAFB7AC-6A9B-44A5-84CE-094E9B5C40EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Completo" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="49">
   <si>
     <t>Tarea</t>
   </si>
@@ -229,11 +229,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1376,7 +1377,7 @@
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10</c:v>
@@ -1385,7 +1386,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>14</c:v>
@@ -1400,7 +1401,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
@@ -1538,7 +1539,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10</c:v>
@@ -1547,7 +1548,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>14</c:v>
@@ -1562,7 +1563,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
@@ -1818,43 +1819,49 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Iteracion 2'!$A$2:$A$13</c:f>
+              <c:f>'Iteracion 2'!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>Desarrollo de la Infraestructura</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Desarrollo de endpoints para los servicios</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Módulo: asistencia</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>Crear generador de códigos QR</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>Acoplar código QR en perfil de asistente y en vista de asistencia</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>Crear vista "Toma de Asistencia"</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>Crear servicio para obtener actividades con asistencia</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>Crear servicio de registro y lectura de códigos QR</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Gestión del Proceso de Desarrollo</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Reuniones con Clientes</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>Deploy: Iteración 2</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Pruebas y Testing</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Pruebas integrales</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>Pruebas de aceptación</c:v>
                 </c:pt>
               </c:strCache>
@@ -1862,10 +1869,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteracion 2'!$B$2:$B$13</c:f>
+              <c:f>'Iteracion 2'!$B$2:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>43636</c:v>
                 </c:pt>
@@ -1873,33 +1880,39 @@
                   <c:v>43636</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>43636</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43636</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>43638</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>43641</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>43643</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>43647</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>43612</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>43612</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>43650</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>43636</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>43636</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>43636</c:v>
                 </c:pt>
               </c:numCache>
@@ -1944,7 +1957,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="6"/>
+            <c:idx val="2"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1956,14 +1969,9 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-397A-4AA8-9A98-ABC07CC0EC26}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="9"/>
+            <c:idx val="8"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1975,51 +1983,66 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-397A-4AA8-9A98-ABC07CC0EC26}"/>
-              </c:ext>
-            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C2514D"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Iteracion 2'!$A$2:$A$13</c:f>
+              <c:f>'Iteracion 2'!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>Desarrollo de la Infraestructura</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Desarrollo de endpoints para los servicios</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Módulo: asistencia</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>Crear generador de códigos QR</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>Acoplar código QR en perfil de asistente y en vista de asistencia</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>Crear vista "Toma de Asistencia"</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>Crear servicio para obtener actividades con asistencia</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>Crear servicio de registro y lectura de códigos QR</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Gestión del Proceso de Desarrollo</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Reuniones con Clientes</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>Deploy: Iteración 2</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Pruebas y Testing</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Pruebas integrales</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>Pruebas de aceptación</c:v>
                 </c:pt>
               </c:strCache>
@@ -2027,44 +2050,50 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteracion 2'!$D$2:$D$13</c:f>
+              <c:f>'Iteracion 2'!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
@@ -7618,8 +7647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D8BD03-6FA3-4BE7-A8B5-8D754451A416}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8406,8 +8435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F541D4-632E-4CF3-82CA-982F795E8F2A}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8437,11 +8466,11 @@
         <v>43612</v>
       </c>
       <c r="C2" s="1">
-        <v>43636</v>
+        <v>43637</v>
       </c>
       <c r="D2">
         <f>C2-B2</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8482,11 +8511,11 @@
         <v>43622</v>
       </c>
       <c r="C5" s="1">
-        <v>43650</v>
+        <v>43637</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -8557,11 +8586,11 @@
         <v>43612</v>
       </c>
       <c r="C10" s="1">
-        <v>43636</v>
+        <v>43637</v>
       </c>
       <c r="D10">
         <f>C10-B10</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -8634,6 +8663,9 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="4"/>
+    </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
@@ -8733,7 +8765,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8741,8 +8774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B17453-26BC-47A2-BB64-4A12FA0B0C8A}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="I4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8766,7 +8799,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>43636</v>
@@ -8775,171 +8808,201 @@
         <v>43650</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D7" si="0">C2-B2</f>
+        <f t="shared" ref="D2:D9" si="0">C2-B2</f>
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>43636</v>
       </c>
       <c r="C3" s="1">
-        <v>43641</v>
+        <v>43650</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>43638</v>
+        <v>43636</v>
       </c>
       <c r="C4" s="1">
-        <v>43641</v>
+        <v>43650</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
+        <v>43636</v>
+      </c>
+      <c r="C5" s="1">
         <v>43641</v>
-      </c>
-      <c r="C5" s="1">
-        <v>43648</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
-        <v>43643</v>
+        <v>43638</v>
       </c>
       <c r="C6" s="1">
-        <v>43648</v>
+        <v>43641</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
-        <v>43647</v>
+        <v>43641</v>
       </c>
       <c r="C7" s="1">
-        <v>43650</v>
+        <v>43648</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
-        <v>43612</v>
+        <v>43643</v>
       </c>
       <c r="C8" s="1">
-        <v>43651</v>
+        <v>43648</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D13" si="1">C8-B8</f>
-        <v>39</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1">
+        <v>43647</v>
+      </c>
+      <c r="C9" s="1">
+        <v>43650</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43612</v>
+      </c>
+      <c r="C10" s="1">
+        <v>43651</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:D15" si="1">C10-B10</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B11" s="1">
         <v>43612</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C11" s="1">
         <v>43651</v>
       </c>
-      <c r="D9">
+      <c r="D11">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B12" s="1">
         <v>43650</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C12" s="1">
         <v>43651</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B13" s="1">
         <v>43636</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C13" s="1">
         <v>43651</v>
       </c>
-      <c r="D11">
+      <c r="D13">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B14" s="1">
         <v>43636</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C14" s="1">
         <v>43651</v>
       </c>
-      <c r="D12">
+      <c r="D14">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B15" s="1">
         <v>43636</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C15" s="1">
         <v>43651</v>
       </c>
-      <c r="D13">
+      <c r="D15">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
@@ -9978,7 +10041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C040AA46-4824-499A-AC6B-49AC956C6EE1}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Actualizados diagramas de gantt para que las fechas se correspondan correctamente a las de las iteraciones
</commit_message>
<xml_diff>
--- a/Informe/Diagrama de Gantt/Diagrama de Gantt.xlsx
+++ b/Informe/Diagrama de Gantt/Diagrama de Gantt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Conferentia\Informe\Diagrama de Gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A2898A-8E9A-4C44-914D-320710E08A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22D3BFE-56D5-44D8-946B-2E8D5FD409CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{5FAFB7AC-6A9B-44A5-84CE-094E9B5C40EE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5FAFB7AC-6A9B-44A5-84CE-094E9B5C40EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Completo" sheetId="1" r:id="rId1"/>
@@ -458,10 +458,10 @@
                   <c:v>43631</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43636</c:v>
+                  <c:v>43637</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43636</c:v>
+                  <c:v>43637</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>43638</c:v>
@@ -476,13 +476,13 @@
                   <c:v>43647</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43650</c:v>
+                  <c:v>43651</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43650</c:v>
+                  <c:v>43651</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43650</c:v>
+                  <c:v>43651</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>43653</c:v>
@@ -500,10 +500,10 @@
                   <c:v>43662</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43667</c:v>
+                  <c:v>43668</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43667</c:v>
+                  <c:v>43668</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>43669</c:v>
@@ -512,16 +512,16 @@
                   <c:v>43673</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43674</c:v>
+                  <c:v>43676</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43674</c:v>
+                  <c:v>43676</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43674</c:v>
+                  <c:v>43676</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>43674</c:v>
+                  <c:v>43676</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>43678</c:v>
@@ -923,10 +923,10 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>3</c:v>
@@ -941,13 +941,13 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>14</c:v>
@@ -965,10 +965,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>5</c:v>
@@ -977,16 +977,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>3</c:v>
@@ -1874,16 +1874,16 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43636</c:v>
+                  <c:v>43637</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43636</c:v>
+                  <c:v>43637</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43636</c:v>
+                  <c:v>43637</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43636</c:v>
+                  <c:v>43637</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>43638</c:v>
@@ -1907,13 +1907,13 @@
                   <c:v>43650</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43636</c:v>
+                  <c:v>43637</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43636</c:v>
+                  <c:v>43637</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43636</c:v>
+                  <c:v>43637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1969,6 +1969,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-8E73-48FE-97D2-200D88DD62E6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -1983,6 +1988,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-8E73-48FE-97D2-200D88DD62E6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -1997,6 +2007,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-8E73-48FE-97D2-200D88DD62E6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -2055,16 +2070,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3</c:v>
@@ -2088,13 +2103,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2202,7 +2217,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43651"/>
-          <c:min val="43636"/>
+          <c:min val="43637"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -2407,13 +2422,13 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43650</c:v>
+                  <c:v>43651</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43650</c:v>
+                  <c:v>43651</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43650</c:v>
+                  <c:v>43651</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>43653</c:v>
@@ -2431,22 +2446,22 @@
                   <c:v>43662</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43650</c:v>
+                  <c:v>43651</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43650</c:v>
+                  <c:v>43651</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>43667</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43650</c:v>
+                  <c:v>43651</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43650</c:v>
+                  <c:v>43651</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43650</c:v>
+                  <c:v>43651</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2603,13 +2618,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>14</c:v>
@@ -2627,22 +2642,22 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2736,7 +2751,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43668"/>
-          <c:min val="43650"/>
+          <c:min val="43651"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -2929,10 +2944,10 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>43667</c:v>
+                  <c:v>43668</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43667</c:v>
+                  <c:v>43668</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>43669</c:v>
@@ -2941,22 +2956,22 @@
                   <c:v>43673</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43667</c:v>
+                  <c:v>43668</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43667</c:v>
+                  <c:v>43668</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>43675</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43667</c:v>
+                  <c:v>43668</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43667</c:v>
+                  <c:v>43668</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43667</c:v>
+                  <c:v>43668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3082,10 +3097,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5</c:v>
@@ -3094,22 +3109,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3203,7 +3218,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43676"/>
-          <c:min val="43667"/>
+          <c:min val="43668"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -3405,16 +3420,16 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>43674</c:v>
+                  <c:v>43676</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43674</c:v>
+                  <c:v>43676</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43674</c:v>
+                  <c:v>43676</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43674</c:v>
+                  <c:v>43676</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>43678</c:v>
@@ -3423,10 +3438,10 @@
                   <c:v>43678</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43674</c:v>
+                  <c:v>43676</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43674</c:v>
+                  <c:v>43676</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>43681</c:v>
@@ -3435,13 +3450,13 @@
                   <c:v>43684</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43674</c:v>
+                  <c:v>43676</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43674</c:v>
+                  <c:v>43676</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43674</c:v>
+                  <c:v>43676</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3576,16 +3591,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3</c:v>
@@ -3594,10 +3609,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
@@ -3606,13 +3621,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3706,7 +3721,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43685"/>
-          <c:min val="43674"/>
+          <c:min val="43676"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -7310,13 +7325,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>219074</xdr:colOff>
+      <xdr:colOff>219073</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>5332</xdr:rowOff>
     </xdr:to>
@@ -7647,8 +7662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D8BD03-6FA3-4BE7-A8B5-8D754451A416}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7795,14 +7810,14 @@
         <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>43636</v>
+        <v>43637</v>
       </c>
       <c r="C10" s="1">
         <v>43650</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7810,14 +7825,14 @@
         <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>43636</v>
+        <v>43637</v>
       </c>
       <c r="C11" s="1">
         <v>43641</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -7885,14 +7900,14 @@
         <v>17</v>
       </c>
       <c r="B16" s="1">
-        <v>43650</v>
+        <v>43651</v>
       </c>
       <c r="C16" s="1">
         <v>43657</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -7900,14 +7915,14 @@
         <v>18</v>
       </c>
       <c r="B17" s="1">
-        <v>43650</v>
+        <v>43651</v>
       </c>
       <c r="C17" s="1">
         <v>43653</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -7915,14 +7930,14 @@
         <v>19</v>
       </c>
       <c r="B18" s="1">
-        <v>43650</v>
+        <v>43651</v>
       </c>
       <c r="C18" s="1">
         <v>43657</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -8005,14 +8020,14 @@
         <v>25</v>
       </c>
       <c r="B24" s="1">
-        <v>43667</v>
+        <v>43668</v>
       </c>
       <c r="C24" s="1">
         <v>43674</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -8020,14 +8035,14 @@
         <v>26</v>
       </c>
       <c r="B25" s="1">
-        <v>43667</v>
+        <v>43668</v>
       </c>
       <c r="C25" s="1">
         <v>43670</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -8065,14 +8080,14 @@
         <v>29</v>
       </c>
       <c r="B28" s="1">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="C28" s="1">
         <v>43681</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -8080,14 +8095,14 @@
         <v>30</v>
       </c>
       <c r="B29" s="1">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="C29" s="1">
         <v>43678</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -8095,14 +8110,14 @@
         <v>31</v>
       </c>
       <c r="B30" s="1">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="C30" s="1">
         <v>43678</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -8110,14 +8125,14 @@
         <v>32</v>
       </c>
       <c r="B31" s="1">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="C31" s="1">
         <v>43678</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -8435,7 +8450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F541D4-632E-4CF3-82CA-982F795E8F2A}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D4" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -8774,8 +8789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B17453-26BC-47A2-BB64-4A12FA0B0C8A}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8802,14 +8817,14 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>43636</v>
+        <v>43637</v>
       </c>
       <c r="C2" s="1">
         <v>43650</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D9" si="0">C2-B2</f>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8817,14 +8832,14 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>43636</v>
+        <v>43637</v>
       </c>
       <c r="C3" s="1">
         <v>43650</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -8832,14 +8847,14 @@
         <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>43636</v>
+        <v>43637</v>
       </c>
       <c r="C4" s="1">
         <v>43650</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -8847,14 +8862,14 @@
         <v>12</v>
       </c>
       <c r="B5" s="1">
-        <v>43636</v>
+        <v>43637</v>
       </c>
       <c r="C5" s="1">
         <v>43641</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -8967,14 +8982,14 @@
         <v>43</v>
       </c>
       <c r="B13" s="1">
-        <v>43636</v>
+        <v>43637</v>
       </c>
       <c r="C13" s="1">
         <v>43651</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -8982,14 +8997,14 @@
         <v>44</v>
       </c>
       <c r="B14" s="1">
-        <v>43636</v>
+        <v>43637</v>
       </c>
       <c r="C14" s="1">
         <v>43651</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -8997,14 +9012,14 @@
         <v>45</v>
       </c>
       <c r="B15" s="1">
-        <v>43636</v>
+        <v>43637</v>
       </c>
       <c r="C15" s="1">
         <v>43651</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -9020,7 +9035,7 @@
         <v>46</v>
       </c>
       <c r="B23" s="2">
-        <v>43636</v>
+        <v>43637</v>
       </c>
       <c r="C23" s="1"/>
     </row>
@@ -9211,8 +9226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AB6520-4DE5-4B14-9F96-39D8B449A877}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD23" sqref="AD23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9239,14 +9254,14 @@
         <v>17</v>
       </c>
       <c r="B2" s="1">
-        <v>43650</v>
+        <v>43651</v>
       </c>
       <c r="C2" s="1">
         <v>43657</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D15" si="0">C2-B2</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -9254,14 +9269,14 @@
         <v>18</v>
       </c>
       <c r="B3" s="1">
-        <v>43650</v>
+        <v>43651</v>
       </c>
       <c r="C3" s="1">
         <v>43653</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -9269,14 +9284,14 @@
         <v>19</v>
       </c>
       <c r="B4" s="1">
-        <v>43650</v>
+        <v>43651</v>
       </c>
       <c r="C4" s="1">
         <v>43657</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -9359,14 +9374,14 @@
         <v>35</v>
       </c>
       <c r="B10" s="1">
-        <v>43650</v>
+        <v>43651</v>
       </c>
       <c r="C10" s="1">
         <v>43668</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -9374,14 +9389,14 @@
         <v>36</v>
       </c>
       <c r="B11" s="1">
-        <v>43650</v>
+        <v>43651</v>
       </c>
       <c r="C11" s="1">
         <v>43668</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -9404,14 +9419,14 @@
         <v>43</v>
       </c>
       <c r="B13" s="1">
-        <v>43650</v>
+        <v>43651</v>
       </c>
       <c r="C13" s="1">
         <v>43668</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -9419,14 +9434,14 @@
         <v>44</v>
       </c>
       <c r="B14" s="1">
-        <v>43650</v>
+        <v>43651</v>
       </c>
       <c r="C14" s="1">
         <v>43668</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -9434,14 +9449,14 @@
         <v>45</v>
       </c>
       <c r="B15" s="1">
-        <v>43650</v>
+        <v>43651</v>
       </c>
       <c r="C15" s="1">
         <v>43668</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -9452,7 +9467,7 @@
         <v>46</v>
       </c>
       <c r="B18" s="2">
-        <v>43650</v>
+        <v>43651</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -9647,8 +9662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5DAE94-0AAC-4B00-83DE-A038FBD6DF23}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9675,14 +9690,14 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>43667</v>
+        <v>43668</v>
       </c>
       <c r="C2" s="1">
         <v>43674</v>
       </c>
       <c r="D2">
         <f>C2-B2</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -9690,14 +9705,14 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>43667</v>
+        <v>43668</v>
       </c>
       <c r="C3" s="1">
         <v>43670</v>
       </c>
       <c r="D3">
         <f>C3-B3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -9735,14 +9750,14 @@
         <v>35</v>
       </c>
       <c r="B6" s="1">
-        <v>43667</v>
+        <v>43668</v>
       </c>
       <c r="C6" s="1">
         <v>43676</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D7" si="0">C6-B6</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -9750,14 +9765,14 @@
         <v>36</v>
       </c>
       <c r="B7" s="1">
-        <v>43667</v>
+        <v>43668</v>
       </c>
       <c r="C7" s="1">
         <v>43676</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -9780,14 +9795,14 @@
         <v>43</v>
       </c>
       <c r="B9" s="1">
-        <v>43667</v>
+        <v>43668</v>
       </c>
       <c r="C9" s="1">
         <v>43676</v>
       </c>
       <c r="D9">
         <f>C9-B9</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -9795,14 +9810,14 @@
         <v>44</v>
       </c>
       <c r="B10" s="1">
-        <v>43667</v>
+        <v>43668</v>
       </c>
       <c r="C10" s="1">
         <v>43676</v>
       </c>
       <c r="D10">
         <f>C10-B10</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -9810,14 +9825,14 @@
         <v>45</v>
       </c>
       <c r="B11" s="1">
-        <v>43667</v>
+        <v>43668</v>
       </c>
       <c r="C11" s="1">
         <v>43676</v>
       </c>
       <c r="D11">
         <f>C11-B11</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -9825,7 +9840,7 @@
         <v>46</v>
       </c>
       <c r="B13" s="2">
-        <v>43667</v>
+        <v>43668</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -10041,8 +10056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C040AA46-4824-499A-AC6B-49AC956C6EE1}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10069,14 +10084,14 @@
         <v>29</v>
       </c>
       <c r="B2" s="1">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="C2" s="1">
         <v>43681</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D14" si="0">C2-B2</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -10084,14 +10099,14 @@
         <v>30</v>
       </c>
       <c r="B3" s="1">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="C3" s="1">
         <v>43678</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -10099,14 +10114,14 @@
         <v>31</v>
       </c>
       <c r="B4" s="1">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="C4" s="1">
         <v>43678</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -10114,14 +10129,14 @@
         <v>32</v>
       </c>
       <c r="B5" s="1">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="C5" s="1">
         <v>43678</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -10159,14 +10174,14 @@
         <v>35</v>
       </c>
       <c r="B8" s="1">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="C8" s="1">
         <v>43685</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -10174,14 +10189,14 @@
         <v>36</v>
       </c>
       <c r="B9" s="1">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="C9" s="1">
         <v>43685</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -10219,14 +10234,14 @@
         <v>43</v>
       </c>
       <c r="B12" s="1">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="C12" s="1">
         <v>43685</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -10234,14 +10249,14 @@
         <v>44</v>
       </c>
       <c r="B13" s="1">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="C13" s="1">
         <v>43681</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -10249,14 +10264,14 @@
         <v>45</v>
       </c>
       <c r="B14" s="1">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="C14" s="1">
         <v>43684</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -10269,7 +10284,7 @@
         <v>46</v>
       </c>
       <c r="B20" s="2">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="C20" s="1"/>
     </row>

</xml_diff>